<commit_message>
cutting some un-needed functions
the old generatedata.py stuff in functions.py
</commit_message>
<xml_diff>
--- a/test_template.xlsx
+++ b/test_template.xlsx
@@ -1,39 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Twig\CS\Python\Stock Data\Stock-Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="2"/>
+    <workbookView activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="CBOE" sheetId="1" r:id="rId1"/>
-    <sheet name="AAPL" sheetId="2" r:id="rId2"/>
-    <sheet name="ACN" sheetId="3" r:id="rId3"/>
+    <sheet name="CBOE" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="AAPL" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ACN" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,24 +49,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -354,37 +345,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>